<commit_message>
added testcases for object repo
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD923607-8E3C-485A-9B90-F0650A2BCD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="4620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +17,11 @@
     <sheet name="HO_ADD_FSG" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="A1:P13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
   <si>
     <t>USER NAME</t>
   </si>
@@ -273,12 +273,15 @@
   </si>
   <si>
     <t>Fosroc@2</t>
+  </si>
+  <si>
+    <t>Distributor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,9 +371,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -408,9 +411,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,7 +448,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,7 +483,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -653,20 +656,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -674,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -682,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -690,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -698,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -706,7 +709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -714,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -722,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -730,35 +733,47 @@
         <v>83</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10001</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{2C765BBD-5063-4964-820B-0E7B5B455C29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -790,7 +805,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -824,31 +839,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="35.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -868,7 +883,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -895,43 +910,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -978,7 +993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1025,7 +1040,7 @@
         <v>440011</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1057,7 +1072,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1091,31 +1106,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1129,7 +1144,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1149,23 +1164,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="2" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1203,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1211,7 +1226,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1234,15 +1249,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new creation changes code
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
   <si>
     <t>USER NAME</t>
   </si>
@@ -272,10 +272,10 @@
     <t>SFA-001</t>
   </si>
   <si>
-    <t>Fosroc@2</t>
-  </si>
-  <si>
     <t>Distributor</t>
+  </si>
+  <si>
+    <t>Raj Kumar</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +730,7 @@
         <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -741,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -769,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,6 +844,11 @@
       </c>
       <c r="J2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new distributor change 13 june
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
   <si>
     <t>USER NAME</t>
   </si>
@@ -275,7 +275,10 @@
     <t>Distributor</t>
   </si>
   <si>
-    <t>Raj Kumar</t>
+    <t>Fosroc@3</t>
+  </si>
+  <si>
+    <t>sahil Khan</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +733,7 @@
         <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -772,7 +775,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,7 +851,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new change 16 june
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEF4C08-E7A4-45DE-927B-C9E511B1F009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,11 +16,12 @@
     <sheet name="HO_ADD_FSG" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
+  <oleSize ref="A1:P14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
   <si>
     <t>USER NAME</t>
   </si>
@@ -275,16 +275,19 @@
     <t>Distributor</t>
   </si>
   <si>
-    <t>Raj Kumar</t>
-  </si>
-  <si>
     <t>Super-9420</t>
+  </si>
+  <si>
+    <t>Fosroc@3</t>
+  </si>
+  <si>
+    <t>ravi varma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,9 +377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -414,9 +417,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,7 +454,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,7 +489,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -659,20 +662,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -688,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -696,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -704,7 +707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -712,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -720,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -728,15 +731,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10001</v>
       </c>
@@ -747,9 +750,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -757,35 +760,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -817,7 +820,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -849,38 +852,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -900,7 +903,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -927,43 +930,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>440011</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1123,31 +1126,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1181,23 +1184,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1266,15 +1269,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F4" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Automation SQL OTP Code Push SECR Developer Cred Class
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66BC722-F3E3-4FFF-AEC8-A9046DFD2BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="4620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,6 @@
     <sheet name="HO_ADD_FSG" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="A1:P14"/>
 </workbook>
 </file>
 
@@ -287,7 +287,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,9 +377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -417,9 +417,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -454,7 +454,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,7 +489,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -662,20 +662,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -691,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -699,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -715,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -723,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -731,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -739,7 +739,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10001</v>
       </c>
@@ -750,7 +750,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -760,35 +760,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -820,7 +820,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -852,38 +852,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -903,7 +903,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -930,43 +930,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>440011</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1126,31 +1126,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1184,23 +1184,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="2" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1269,15 +1269,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
9 july add features
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB7F963-4438-4363-B1FE-9B8A07ACF29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16596" windowHeight="7884"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +17,7 @@
     <sheet name="HO_ADD_FSG" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
+  <oleSize ref="A1:O25"/>
 </workbook>
 </file>
 
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -381,9 +381,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -421,9 +421,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,7 +458,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,7 +493,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -666,20 +666,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -695,7 +695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -711,7 +711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -719,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -727,7 +727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -735,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -743,7 +743,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10001</v>
       </c>
@@ -754,7 +754,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -764,33 +764,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99A350E-0EDC-4561-8BF0-53D199EB3446}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -808,28 +808,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{2B507BF4-3EA1-4A21-B16C-04197E852E28}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -861,7 +861,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -893,38 +893,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -944,7 +944,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -971,43 +971,43 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>440011</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1167,31 +1167,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1225,23 +1225,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1310,15 +1310,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F4" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
10 july add new code
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16596" windowHeight="7884"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t>USER NAME</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>SECR-00800</t>
+  </si>
+  <si>
+    <t>Fosroc@9</t>
   </si>
 </sst>
 </file>
@@ -670,7 +673,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,7 +735,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add features 16 july
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="4620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15924" windowHeight="4620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="HO_ADD_FSG" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="A1:O25"/>
+  <oleSize ref="A1:N14"/>
 </workbook>
 </file>
 
@@ -255,9 +255,6 @@
     <t>YTD Sles</t>
   </si>
   <si>
-    <t>Vinay Thakur</t>
-  </si>
-  <si>
     <t>vinaythakur5420@gmail.com</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>Fosroc@9</t>
+  </si>
+  <si>
+    <t>Tannu sharma</t>
   </si>
 </sst>
 </file>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,18 +732,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -754,12 +754,12 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,22 +866,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2">
+        <v>8745995210</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B2">
-        <v>8745965210</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
       </c>
       <c r="E2">
         <v>411041</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new changes 12 -08
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248FA476-3A09-4AC8-A5E4-A6087BCCE080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AA009C-1B3B-4DF3-969E-2CB06BE07C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
   <si>
     <t>USER NAME</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Fosroc@6</t>
+  </si>
+  <si>
+    <t>Web login SECR</t>
   </si>
 </sst>
 </file>
@@ -670,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,6 +768,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -775,6 +789,7 @@
     <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{A1C1686E-419B-4243-9510-F719A1B4724B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Password update SECR web & mobile
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AA009C-1B3B-4DF3-969E-2CB06BE07C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BCA207-300B-4CA9-8FC8-9DE2D038D248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t>USER NAME</t>
   </si>
@@ -288,10 +288,16 @@
     <t>pranamaya Thakur</t>
   </si>
   <si>
-    <t>Fosroc@6</t>
-  </si>
-  <si>
     <t>Web login SECR</t>
+  </si>
+  <si>
+    <t>Fosroc@7</t>
+  </si>
+  <si>
+    <t>Fosroc@4</t>
+  </si>
+  <si>
+    <t>Fosroc@0</t>
   </si>
 </sst>
 </file>
@@ -676,7 +682,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +728,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,7 +744,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,10 +779,10 @@
         <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new xpath for login btn
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_FSRC.xlsx
+++ b/Excel_TestData/Excel_FSRC.xlsx
@@ -288,13 +288,13 @@
     <t>pranamaya Thakur</t>
   </si>
   <si>
-    <t>Fosroc@6</t>
-  </si>
-  <si>
-    <t>Fosroc@5</t>
-  </si>
-  <si>
     <t>Web login SECR</t>
+  </si>
+  <si>
+    <t>Fosroc@0</t>
+  </si>
+  <si>
+    <t>Fosroc@7</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +725,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -741,7 +741,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -779,7 +779,7 @@
         <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>